<commit_message>
Created an actual test plan - renamed old test plan to test scenario
</commit_message>
<xml_diff>
--- a/WynikiTestow.xlsx
+++ b/WynikiTestow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KUBA\PROJECTS\TestujSystell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A17CFC2F-45D1-4569-9716-F527391CB964}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F4FFFC6-8CBD-43F8-A0CF-182E7C6002E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
   <si>
     <t>Numer testu</t>
   </si>
@@ -85,13 +85,16 @@
   </si>
   <si>
     <t>Błędny wynik</t>
+  </si>
+  <si>
+    <t>NR - Not Run, P - Passed, F - Failed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,6 +133,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -161,7 +173,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -199,15 +211,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -236,11 +258,18 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="20% - Accent1" xfId="3" builtinId="30"/>
     <cellStyle name="60% - Accent1" xfId="4" builtinId="32"/>
     <cellStyle name="Check Cell" xfId="2" builtinId="23"/>
+    <cellStyle name="Explanatory Text" xfId="5" builtinId="53"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -520,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:E9"/>
+  <dimension ref="B1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,9 +560,10 @@
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="12.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="86.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="6" width="31.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -649,7 +679,16 @@
         <v>18</v>
       </c>
     </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D10" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="11"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D10:E10"/>
+  </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>